<commit_message>
Updated the table about generics. Fixed performance section and moved it before the usage examples. Added some figures and IEEE style sheets.
</commit_message>
<xml_diff>
--- a/TUT/ip.hwp.communication/hibi/doc/Datasheet/Fig/tables.xlsx
+++ b/TUT/ip.hwp.communication/hibi/doc/Datasheet/Fig/tables.xlsx
@@ -4,22 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="19980" windowHeight="8325" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="19980" windowHeight="8325"/>
   </bookViews>
   <sheets>
-    <sheet name="hibiv1_vs_hibiv2 Phd '10" sheetId="1" r:id="rId1"/>
-    <sheet name="hibi v3 datasheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="generic params of hibi" sheetId="5" r:id="rId1"/>
+    <sheet name="hibiv1_vs_hibiv2 Phd '10" sheetId="1" r:id="rId2"/>
+    <sheet name="hibi v3 datasheet" sheetId="2" r:id="rId3"/>
+    <sheet name="performance" sheetId="3" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="281">
   <si>
     <t>Property</t>
   </si>
@@ -584,9 +582,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>measure</t>
-  </si>
-  <si>
     <t>bytes</t>
   </si>
   <si>
@@ -597,16 +592,347 @@
   </si>
   <si>
     <t>byte/s</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Mbyte/s</t>
+  </si>
+  <si>
+    <t>Juha Arvio, November 2011</t>
+  </si>
+  <si>
+    <t>HIBI wrapper generics</t>
+  </si>
+  <si>
+    <t>Created by</t>
+  </si>
+  <si>
+    <t>Erno Salminen, Timo Hämäläinen</t>
+  </si>
+  <si>
+    <t>HIBI wrapper r2 is not in use.</t>
+  </si>
+  <si>
+    <t>Kactus (default) settings override VHDL defaults.</t>
+  </si>
+  <si>
+    <t>All generics are of type integer.</t>
+  </si>
+  <si>
+    <t>Generic and VHDL default</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Value range</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Entry in Kactus</t>
+  </si>
+  <si>
+    <t>addr_width_g : integer := 32;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structural </t>
+  </si>
+  <si>
+    <t>Bus widths</t>
+  </si>
+  <si>
+    <t>Bits</t>
+  </si>
+  <si>
+    <t>N/A currently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_width_g : integer := 32; </t>
+  </si>
+  <si>
+    <t>positive integer</t>
+  </si>
+  <si>
+    <t>practically always 3</t>
+  </si>
+  <si>
+    <t>width of command bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counter_width_g : integer := 8; </t>
+  </si>
+  <si>
+    <t>greater or equal than (log(max_send)</t>
+  </si>
+  <si>
+    <t>width if the internal counters in a wrapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debug_width_g : integer := 0 </t>
+  </si>
+  <si>
+    <t>width of debug port (for special monitors)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rx_fifo_depth_g : integer := 5; </t>
+  </si>
+  <si>
+    <t>FIFO</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>0,2,3…</t>
+  </si>
+  <si>
+    <t>Rx fifo depth</t>
+  </si>
+  <si>
+    <t>Must be set manually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rx_msg_fifo_depth_g : integer := 5; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx_fifo_depth_g : integer := 5; </t>
+  </si>
+  <si>
+    <t>Tx fifo depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx_msg_fifo_depth_g : integer := 5; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fifo_sel_g : integer := 0; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronization </t>
+  </si>
+  <si>
+    <t>Clock domains</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Type of the synchronizing FIFO buffers between bus and agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rel_agent_freq_g : integer := 1; </t>
+  </si>
+  <si>
+    <t>Relative frequencies of IP and bus, Needed at least for synchr. multiclk FIFOs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rel_bus_freq_g : integer := 1; </t>
+  </si>
+  <si>
+    <t>see above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addr_g : integer := 46; </t>
+  </si>
+  <si>
+    <t>Addressing</t>
+  </si>
+  <si>
+    <t>unique address for each wrapper</t>
+  </si>
+  <si>
+    <t>Automatically set by generators, override VHDL defaults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv_addr_en_g : integer := 0; </t>
+  </si>
+  <si>
+    <t>0 or 1</t>
+  </si>
+  <si>
+    <t>only for bridges, other half uses 0 and the other 1</t>
+  </si>
+  <si>
+    <t>multicast_en_g : integer := 0</t>
+  </si>
+  <si>
+    <t>enable special addressing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_agents_g : integer := 4; </t>
+  </si>
+  <si>
+    <t>Arbitration</t>
+  </si>
+  <si>
+    <t>total number of agents within one segment (distributed arbitration requires this)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prior_g : integer := 2; </t>
+  </si>
+  <si>
+    <t>less than or equal n_agents</t>
+  </si>
+  <si>
+    <t>unique priority value for all wrappers within one segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_send_g : integer := 50; </t>
+  </si>
+  <si>
+    <t>in words, 0 means unlimited</t>
+  </si>
+  <si>
+    <t>max words the wrapper can reserve bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_time_slots_g : integer := 0; </t>
+  </si>
+  <si>
+    <t>Number of time slots in a TDMA frame. TDMA is enabled by setting n_time_slots &gt; 0. Ensure that all wrappers in a segment agree on arb_type, n_agents, and n_slots. Max_send can be wrapper-specific.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arb_type_g : integer := 0; </t>
+  </si>
+  <si>
+    <t>0 round-robin, 1 priority, 2 combined, 3 DAA</t>
+  </si>
+  <si>
+    <t>Arbitration type</t>
+  </si>
+  <si>
+    <t>keep_slot_g := 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For TDMA: 0 release unused time slots 1 keep unused slots </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Keep reserved but unused slots in TDMA. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Not used in HIBI revision r3</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">id_g : integer := 5; </t>
+  </si>
+  <si>
+    <t>Reconfiguration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_width_g : integer := 4; </t>
+  </si>
+  <si>
+    <t>greater than or equal(log2(id_g))</t>
+  </si>
+  <si>
+    <t>wrapper identification size = max number of wrappers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_id_g : integer := 5; </t>
+  </si>
+  <si>
+    <t>only for bridges, which cfg id are routed acrossa the bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_re_g : integer := 0; </t>
+  </si>
+  <si>
+    <t>enable reading configuration memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_we_g : integer := 0; </t>
+  </si>
+  <si>
+    <t>enable writing configuration memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_extra_params_g : integer := 0; </t>
+  </si>
+  <si>
+    <t>Number of app-specific extra registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_cfg_pages_g : integer := 1; </t>
+  </si>
+  <si>
+    <t>1,2,3...</t>
+  </si>
+  <si>
+    <t>Number of configuration pages. Having multiple pages allows fast reconfig. Note that cfg memory initialization is done with separate  package if you have many time slots or configuration pages</t>
+  </si>
+  <si>
+    <t>Table copied from \\vault.dcs.cs.tut.fi\PROJECTS\FunBase\Funbase IP blocks\HIBI\HIBI configuration parameters.xlsx on 2011-11-15</t>
+  </si>
+  <si>
+    <t>Func/Struct</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>less than or equal data_width_g if muxed</t>
+  </si>
+  <si>
+    <t>address (bus) width</t>
+  </si>
+  <si>
+    <t>width of data bus (which can be multiplexed with address)</t>
+  </si>
+  <si>
+    <t>comm_width_g : integer := 5;</t>
+  </si>
+  <si>
+    <t>Rx message (high-priority) fifo depth</t>
+  </si>
+  <si>
+    <t>Tx message (high-priority) fifo depth</t>
+  </si>
+  <si>
+    <t>0-3:  Synchronous multi-clock,
+GALS  (globally asynchronous, locally synchronous),
+Gray FIFO, or
+Mixed clock pausible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique wrapper identification for reconfiguration </t>
+  </si>
+  <si>
+    <t>Functional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -657,8 +983,45 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -683,6 +1046,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -1072,95 +1441,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1169,149 +1539,243 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1322,9 +1786,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1364,7 +1826,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$15</c:f>
+              <c:f>performance!$C$6:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1403,7 +1865,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$6:$E$15</c:f>
+              <c:f>performance!$E$6:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1441,11 +1903,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="116260864"/>
-        <c:axId val="116262400"/>
+        <c:axId val="113867392"/>
+        <c:axId val="113886720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116260864"/>
+        <c:axId val="113867392"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1462,7 +1924,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Wrapper fifo size / words</a:t>
+                  <a:t>Wrapper fifo depth,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[words]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1471,12 +1941,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116262400"/>
+        <c:crossAx val="113886720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116262400"/>
+        <c:axId val="113886720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,30 +1967,33 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> time / cycles</a:t>
+                  <a:t> time, [cycles]</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="4.5819006625897373E-3"/>
+              <c:y val="0.20113573432186957"/>
+            </c:manualLayout>
+          </c:layout>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116260864"/>
+        <c:crossAx val="113867392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1530,9 +2003,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1572,7 +2043,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$15</c:f>
+              <c:f>performance!$C$6:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1611,49 +2082,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$6:$G$15</c:f>
+              <c:f>performance!$H$6:$H$15</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>443530048.7276665</c:v>
+                  <c:v>443.5300487276665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>512000000</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>691308016.87763715</c:v>
+                  <c:v>691.3080168776371</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>701369863.01369858</c:v>
+                  <c:v>701.36986301369859</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>693649449.61896694</c:v>
+                  <c:v>693.64944961896697</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>694237288.13559318</c:v>
+                  <c:v>694.23728813559319</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>701970865.46700943</c:v>
+                  <c:v>701.97086546700939</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>697191489.36170208</c:v>
+                  <c:v>697.19148936170211</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>735368043.08797133</c:v>
+                  <c:v>735.36804308797127</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>760631383.47260904</c:v>
+                  <c:v>760.63138347260906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="121181696"/>
-        <c:axId val="121422592"/>
+        <c:axId val="117703808"/>
+        <c:axId val="117706112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121181696"/>
+        <c:axId val="117703808"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1670,7 +2141,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Wrapper fifo size / words</a:t>
+                  <a:t>Wrapper fifo depth, [words]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1679,12 +2150,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121422592"/>
+        <c:crossAx val="117706112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121422592"/>
+        <c:axId val="117706112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,34 +2172,37 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Throughput</a:t>
+                  <a:t>Throughput, [M</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> / bytes/s</a:t>
+                  <a:t>Bytes/s]</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0"/>
+              <c:y val="0.20273939984306086"/>
+            </c:manualLayout>
+          </c:layout>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121181696"/>
+        <c:crossAx val="117703808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1849,106 +2323,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1 (2)"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="A1">
-            <v>4</v>
-          </cell>
-          <cell r="B1">
-            <v>1847</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>5</v>
-          </cell>
-          <cell r="B2">
-            <v>1600</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>6</v>
-          </cell>
-          <cell r="B3">
-            <v>1185</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>7</v>
-          </cell>
-          <cell r="B4">
-            <v>1168</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>8</v>
-          </cell>
-          <cell r="B5">
-            <v>1181</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>9</v>
-          </cell>
-          <cell r="B6">
-            <v>1180</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>10</v>
-          </cell>
-          <cell r="B7">
-            <v>1167</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>11</v>
-          </cell>
-          <cell r="B8">
-            <v>1175</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>64</v>
-          </cell>
-          <cell r="B9">
-            <v>1114</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>256</v>
-          </cell>
-          <cell r="B10">
-            <v>1077</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2236,9 +2610,895 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="93"/>
+    <col min="2" max="2" width="5" style="93" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="122" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" style="95" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="95" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" style="95" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" style="96" customWidth="1"/>
+    <col min="9" max="9" width="26" style="96" customWidth="1"/>
+    <col min="10" max="10" width="19" style="97" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="93"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10">
+      <c r="C1" s="94" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10">
+      <c r="C2" s="94" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="C3" s="94" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="C4" s="94" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="C5" s="94"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="C6" s="98" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="C7" s="98" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="C8" s="98" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" s="102" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B9" s="124" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="99" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="100" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" s="100" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" s="100" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="100" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="100" t="s">
+        <v>192</v>
+      </c>
+      <c r="I9" s="100" t="s">
+        <v>193</v>
+      </c>
+      <c r="J9" s="101"/>
+    </row>
+    <row r="10" spans="2:10" ht="26.25" thickTop="1">
+      <c r="B10" s="103">
+        <v>1</v>
+      </c>
+      <c r="C10" s="104" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="105" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="G10" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="H10" s="106" t="s">
+        <v>273</v>
+      </c>
+      <c r="I10" s="107" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="25.5">
+      <c r="B11" s="103">
+        <f>B10+1</f>
+        <v>2</v>
+      </c>
+      <c r="C11" s="104" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="105" t="s">
+        <v>196</v>
+      </c>
+      <c r="F11" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="G11" s="105" t="s">
+        <v>200</v>
+      </c>
+      <c r="H11" s="106" t="s">
+        <v>274</v>
+      </c>
+      <c r="I11" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="103">
+        <f t="shared" ref="B12:B37" si="0">B11+1</f>
+        <v>3</v>
+      </c>
+      <c r="C12" s="104" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="105" t="s">
+        <v>196</v>
+      </c>
+      <c r="F12" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="G12" s="106" t="s">
+        <v>201</v>
+      </c>
+      <c r="H12" s="106" t="s">
+        <v>202</v>
+      </c>
+      <c r="I12" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="25.5">
+      <c r="B13" s="103">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="104" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" s="105" t="s">
+        <v>196</v>
+      </c>
+      <c r="F13" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="G13" s="106" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="I13" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="25.5">
+      <c r="B14" s="108">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="109" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="110" t="s">
+        <v>195</v>
+      </c>
+      <c r="E14" s="110" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" s="110" t="s">
+        <v>197</v>
+      </c>
+      <c r="G14" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="H14" s="110" t="s">
+        <v>207</v>
+      </c>
+      <c r="I14" s="110" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="25.5">
+      <c r="B15" s="103">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="104" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E15" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="F15" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="G15" s="105" t="s">
+        <v>211</v>
+      </c>
+      <c r="H15" s="106" t="s">
+        <v>212</v>
+      </c>
+      <c r="I15" s="111" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="25.5">
+      <c r="B16" s="103">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="104" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E16" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="F16" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="G16" s="105" t="s">
+        <v>211</v>
+      </c>
+      <c r="H16" s="106" t="s">
+        <v>276</v>
+      </c>
+      <c r="I16" s="111" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="25.5">
+      <c r="B17" s="103">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="104" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="G17" s="105" t="s">
+        <v>211</v>
+      </c>
+      <c r="H17" s="106" t="s">
+        <v>216</v>
+      </c>
+      <c r="I17" s="111" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B18" s="103">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C18" s="104" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="F18" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="G18" s="105" t="s">
+        <v>211</v>
+      </c>
+      <c r="H18" s="106" t="s">
+        <v>277</v>
+      </c>
+      <c r="I18" s="111" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" s="97" customFormat="1" ht="63.75">
+      <c r="B19" s="112">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C19" s="113" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" s="114" t="s">
+        <v>219</v>
+      </c>
+      <c r="E19" s="114" t="s">
+        <v>220</v>
+      </c>
+      <c r="F19" s="114" t="s">
+        <v>221</v>
+      </c>
+      <c r="G19" s="125" t="s">
+        <v>278</v>
+      </c>
+      <c r="H19" s="114" t="s">
+        <v>222</v>
+      </c>
+      <c r="I19" s="114" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" s="97" customFormat="1" ht="38.25">
+      <c r="B20" s="115">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C20" s="116" t="s">
+        <v>223</v>
+      </c>
+      <c r="D20" s="117" t="s">
+        <v>219</v>
+      </c>
+      <c r="E20" s="117" t="s">
+        <v>220</v>
+      </c>
+      <c r="F20" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="G20" s="117" t="s">
+        <v>200</v>
+      </c>
+      <c r="H20" s="118" t="s">
+        <v>224</v>
+      </c>
+      <c r="I20" s="118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B21" s="115">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C21" s="116" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" s="117" t="s">
+        <v>219</v>
+      </c>
+      <c r="E21" s="117" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="G21" s="117" t="s">
+        <v>200</v>
+      </c>
+      <c r="H21" s="118" t="s">
+        <v>226</v>
+      </c>
+      <c r="I21" s="118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" s="97" customFormat="1" ht="38.25">
+      <c r="B22" s="103">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="104" t="s">
+        <v>227</v>
+      </c>
+      <c r="D22" s="105" t="s">
+        <v>280</v>
+      </c>
+      <c r="E22" s="105" t="s">
+        <v>228</v>
+      </c>
+      <c r="F22" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G22" s="105" t="s">
+        <v>200</v>
+      </c>
+      <c r="H22" s="106" t="s">
+        <v>229</v>
+      </c>
+      <c r="I22" s="111" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B23" s="103">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C23" s="104" t="s">
+        <v>231</v>
+      </c>
+      <c r="D23" s="105" t="s">
+        <v>280</v>
+      </c>
+      <c r="E23" s="105" t="s">
+        <v>228</v>
+      </c>
+      <c r="F23" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G23" s="104" t="s">
+        <v>232</v>
+      </c>
+      <c r="H23" s="106" t="s">
+        <v>233</v>
+      </c>
+      <c r="I23" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" s="97" customFormat="1">
+      <c r="B24" s="108">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C24" s="109" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="110" t="s">
+        <v>280</v>
+      </c>
+      <c r="E24" s="110" t="s">
+        <v>228</v>
+      </c>
+      <c r="F24" s="110" t="s">
+        <v>221</v>
+      </c>
+      <c r="G24" s="109" t="s">
+        <v>232</v>
+      </c>
+      <c r="H24" s="110" t="s">
+        <v>235</v>
+      </c>
+      <c r="I24" s="110" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" s="97" customFormat="1" ht="38.25">
+      <c r="B25" s="115">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C25" s="116" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" s="117" t="s">
+        <v>280</v>
+      </c>
+      <c r="E25" s="117" t="s">
+        <v>237</v>
+      </c>
+      <c r="F25" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" s="117" t="s">
+        <v>200</v>
+      </c>
+      <c r="H25" s="118" t="s">
+        <v>238</v>
+      </c>
+      <c r="I25" s="119" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B26" s="115">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="117" t="s">
+        <v>280</v>
+      </c>
+      <c r="E26" s="117" t="s">
+        <v>237</v>
+      </c>
+      <c r="F26" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="G26" s="118" t="s">
+        <v>240</v>
+      </c>
+      <c r="H26" s="118" t="s">
+        <v>241</v>
+      </c>
+      <c r="I26" s="119" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" s="97" customFormat="1">
+      <c r="B27" s="115">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C27" s="116" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27" s="117" t="s">
+        <v>280</v>
+      </c>
+      <c r="E27" s="117" t="s">
+        <v>237</v>
+      </c>
+      <c r="F27" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="G27" s="118" t="s">
+        <v>243</v>
+      </c>
+      <c r="H27" s="118" t="s">
+        <v>244</v>
+      </c>
+      <c r="I27" s="118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" s="97" customFormat="1" ht="76.5">
+      <c r="B28" s="115">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C28" s="116" t="s">
+        <v>245</v>
+      </c>
+      <c r="D28" s="117" t="s">
+        <v>280</v>
+      </c>
+      <c r="E28" s="117" t="s">
+        <v>237</v>
+      </c>
+      <c r="F28" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="G28" s="116"/>
+      <c r="H28" s="118" t="s">
+        <v>246</v>
+      </c>
+      <c r="I28" s="118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B29" s="112">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C29" s="113" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" s="114" t="s">
+        <v>280</v>
+      </c>
+      <c r="E29" s="114" t="s">
+        <v>237</v>
+      </c>
+      <c r="F29" s="114" t="s">
+        <v>221</v>
+      </c>
+      <c r="G29" s="114" t="s">
+        <v>248</v>
+      </c>
+      <c r="H29" s="114" t="s">
+        <v>249</v>
+      </c>
+      <c r="I29" s="114" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B30" s="115">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C30" s="116" t="s">
+        <v>250</v>
+      </c>
+      <c r="D30" s="117" t="s">
+        <v>280</v>
+      </c>
+      <c r="E30" s="117" t="s">
+        <v>237</v>
+      </c>
+      <c r="F30" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="G30" s="116" t="s">
+        <v>251</v>
+      </c>
+      <c r="H30" s="118" t="s">
+        <v>252</v>
+      </c>
+      <c r="I30" s="118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B31" s="103">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C31" s="104" t="s">
+        <v>253</v>
+      </c>
+      <c r="D31" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="105" t="s">
+        <v>254</v>
+      </c>
+      <c r="F31" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G31" s="105" t="s">
+        <v>200</v>
+      </c>
+      <c r="H31" s="106" t="s">
+        <v>279</v>
+      </c>
+      <c r="I31" s="111" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B32" s="103">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C32" s="104" t="s">
+        <v>255</v>
+      </c>
+      <c r="D32" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="E32" s="105" t="s">
+        <v>254</v>
+      </c>
+      <c r="F32" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G32" s="105" t="s">
+        <v>256</v>
+      </c>
+      <c r="H32" s="106" t="s">
+        <v>257</v>
+      </c>
+      <c r="I32" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" s="97" customFormat="1" ht="25.5">
+      <c r="B33" s="103">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C33" s="104" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="E33" s="105" t="s">
+        <v>254</v>
+      </c>
+      <c r="F33" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G33" s="105" t="s">
+        <v>200</v>
+      </c>
+      <c r="H33" s="106" t="s">
+        <v>259</v>
+      </c>
+      <c r="I33" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" s="97" customFormat="1">
+      <c r="B34" s="108">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C34" s="109" t="s">
+        <v>260</v>
+      </c>
+      <c r="D34" s="110" t="s">
+        <v>270</v>
+      </c>
+      <c r="E34" s="110" t="s">
+        <v>254</v>
+      </c>
+      <c r="F34" s="110" t="s">
+        <v>221</v>
+      </c>
+      <c r="G34" s="109" t="s">
+        <v>232</v>
+      </c>
+      <c r="H34" s="110" t="s">
+        <v>261</v>
+      </c>
+      <c r="I34" s="110" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" s="97" customFormat="1">
+      <c r="B35" s="103">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C35" s="104" t="s">
+        <v>262</v>
+      </c>
+      <c r="D35" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="E35" s="105" t="s">
+        <v>254</v>
+      </c>
+      <c r="F35" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G35" s="104" t="s">
+        <v>232</v>
+      </c>
+      <c r="H35" s="106" t="s">
+        <v>263</v>
+      </c>
+      <c r="I35" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" s="97" customFormat="1">
+      <c r="B36" s="103">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C36" s="104" t="s">
+        <v>264</v>
+      </c>
+      <c r="D36" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="E36" s="105" t="s">
+        <v>254</v>
+      </c>
+      <c r="F36" s="105" t="s">
+        <v>221</v>
+      </c>
+      <c r="G36" s="105" t="s">
+        <v>200</v>
+      </c>
+      <c r="H36" s="106" t="s">
+        <v>265</v>
+      </c>
+      <c r="I36" s="106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" s="97" customFormat="1" ht="76.5">
+      <c r="B37" s="108">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C37" s="109" t="s">
+        <v>266</v>
+      </c>
+      <c r="D37" s="110" t="s">
+        <v>270</v>
+      </c>
+      <c r="E37" s="110" t="s">
+        <v>254</v>
+      </c>
+      <c r="F37" s="110" t="s">
+        <v>221</v>
+      </c>
+      <c r="G37" s="109" t="s">
+        <v>267</v>
+      </c>
+      <c r="H37" s="110" t="s">
+        <v>268</v>
+      </c>
+      <c r="I37" s="110" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" s="97" customFormat="1">
+      <c r="B38" s="103"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="121"/>
+      <c r="G38" s="121"/>
+      <c r="H38" s="96"/>
+      <c r="I38" s="96"/>
+    </row>
+    <row r="39" spans="2:9" s="97" customFormat="1">
+      <c r="B39" s="103"/>
+      <c r="C39" s="122"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="95"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="96"/>
+    </row>
+    <row r="40" spans="2:9" s="97" customFormat="1">
+      <c r="B40" s="103"/>
+      <c r="C40" s="122"/>
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="96"/>
+    </row>
+    <row r="41" spans="2:9" s="97" customFormat="1">
+      <c r="B41" s="123"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="95"/>
+      <c r="E41" s="95"/>
+      <c r="F41" s="95"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="96"/>
+      <c r="I41" s="96"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:E65"/>
     </sheetView>
   </sheetViews>
@@ -2285,10 +3545,10 @@
     </row>
     <row r="5" spans="1:11" ht="13.5" thickBot="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2302,7 +3562,7 @@
     </row>
     <row r="6" spans="1:11" ht="13.5" thickTop="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="80" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6"/>
@@ -2313,7 +3573,7 @@
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="62"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
@@ -2330,7 +3590,7 @@
     </row>
     <row r="8" spans="1:11" ht="25.5">
       <c r="A8" s="2"/>
-      <c r="B8" s="62"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
@@ -2350,8 +3610,8 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="66" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="83" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -2367,8 +3627,8 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="68"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="17" t="s">
         <v>16</v>
       </c>
@@ -2380,8 +3640,8 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="66" t="s">
+      <c r="B11" s="81"/>
+      <c r="C11" s="83" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -2397,8 +3657,8 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="68"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="84"/>
       <c r="D12" s="17" t="s">
         <v>20</v>
       </c>
@@ -2412,7 +3672,7 @@
     </row>
     <row r="13" spans="1:11" ht="25.5">
       <c r="A13" s="2"/>
-      <c r="B13" s="62"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="15" t="s">
         <v>23</v>
       </c>
@@ -2429,7 +3689,7 @@
     </row>
     <row r="14" spans="1:11" ht="25.5" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="21" t="s">
         <v>26</v>
       </c>
@@ -2446,7 +3706,7 @@
     </row>
     <row r="15" spans="1:11" ht="12.75" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="85" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="9"/>
@@ -2457,7 +3717,7 @@
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="62"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="19" t="s">
         <v>28</v>
       </c>
@@ -2474,8 +3734,8 @@
     </row>
     <row r="17" spans="1:7" ht="38.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="66" t="s">
+      <c r="B17" s="81"/>
+      <c r="C17" s="83" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="24" t="s">
@@ -2491,8 +3751,8 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="67"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="10" t="s">
         <v>36</v>
       </c>
@@ -2506,8 +3766,8 @@
     </row>
     <row r="19" spans="1:7" ht="51">
       <c r="A19" s="2"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="68"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="84"/>
       <c r="D19" s="25" t="s">
         <v>35</v>
       </c>
@@ -2521,8 +3781,8 @@
     </row>
     <row r="20" spans="1:7" ht="25.5">
       <c r="A20" s="2"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="67" t="s">
+      <c r="B20" s="81"/>
+      <c r="C20" s="86" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -2538,8 +3798,8 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="67"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="10" t="s">
         <v>43</v>
       </c>
@@ -2553,8 +3813,8 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="67"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="86"/>
       <c r="D22" s="10" t="s">
         <v>45</v>
       </c>
@@ -2568,8 +3828,8 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="67"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="86"/>
       <c r="D23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2583,8 +3843,8 @@
     </row>
     <row r="24" spans="1:7" ht="25.5">
       <c r="A24" s="2"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="67"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="10" t="s">
         <v>16</v>
       </c>
@@ -2598,8 +3858,8 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="69"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="87"/>
       <c r="D25" s="26" t="s">
         <v>16</v>
       </c>
@@ -2613,7 +3873,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2"/>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="85" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="23"/>
@@ -2624,8 +3884,8 @@
     </row>
     <row r="27" spans="1:7" ht="12.75" customHeight="1">
       <c r="A27" s="2"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="67" t="s">
+      <c r="B27" s="81"/>
+      <c r="C27" s="86" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="11" t="s">
@@ -2641,8 +3901,8 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="68"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="84"/>
       <c r="D28" s="17" t="s">
         <v>57</v>
       </c>
@@ -2656,7 +3916,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2"/>
-      <c r="B29" s="62"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="13" t="s">
         <v>59</v>
       </c>
@@ -2673,7 +3933,7 @@
     </row>
     <row r="30" spans="1:7" ht="25.5">
       <c r="A30" s="2"/>
-      <c r="B30" s="62"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="13" t="s">
         <v>63</v>
       </c>
@@ -2690,7 +3950,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2"/>
-      <c r="B31" s="62"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="13" t="s">
         <v>67</v>
       </c>
@@ -2707,8 +3967,8 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="64" t="s">
+      <c r="B32" s="81"/>
+      <c r="C32" s="88" t="s">
         <v>69</v>
       </c>
       <c r="D32" s="11">
@@ -2724,8 +3984,8 @@
     </row>
     <row r="33" spans="1:7" ht="38.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="64"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="88"/>
       <c r="D33" s="11" t="s">
         <v>71</v>
       </c>
@@ -2739,8 +3999,8 @@
     </row>
     <row r="34" spans="1:7" ht="25.5">
       <c r="A34" s="2"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="70"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="90"/>
       <c r="D34" s="22" t="s">
         <v>73</v>
       </c>
@@ -2754,7 +4014,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2"/>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="85" t="s">
         <v>76</v>
       </c>
       <c r="C35" s="9"/>
@@ -2765,8 +4025,8 @@
     </row>
     <row r="36" spans="1:7" ht="12.75" customHeight="1">
       <c r="A36" s="2"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="64" t="s">
+      <c r="B36" s="81"/>
+      <c r="C36" s="88" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="11" t="s">
@@ -2782,8 +4042,8 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="64"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="88"/>
       <c r="D37" s="11" t="s">
         <v>80</v>
       </c>
@@ -2797,8 +4057,8 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="64"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="88"/>
       <c r="D38" s="11" t="s">
         <v>83</v>
       </c>
@@ -2812,8 +4072,8 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="64"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="88"/>
       <c r="D39" s="11" t="s">
         <v>84</v>
       </c>
@@ -2827,8 +4087,8 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="65"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="89"/>
       <c r="D40" s="17" t="s">
         <v>16</v>
       </c>
@@ -2842,7 +4102,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2"/>
-      <c r="B41" s="62"/>
+      <c r="B41" s="81"/>
       <c r="C41" s="13" t="s">
         <v>87</v>
       </c>
@@ -2859,7 +4119,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2"/>
-      <c r="B42" s="62"/>
+      <c r="B42" s="81"/>
       <c r="C42" s="13" t="s">
         <v>91</v>
       </c>
@@ -2876,7 +4136,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2"/>
-      <c r="B43" s="63"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="27" t="s">
         <v>95</v>
       </c>
@@ -2893,7 +4153,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="2"/>
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="85" t="s">
         <v>99</v>
       </c>
       <c r="C44" s="23"/>
@@ -2904,8 +4164,8 @@
     </row>
     <row r="45" spans="1:7" ht="25.5" customHeight="1">
       <c r="A45" s="2"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="67" t="s">
+      <c r="B45" s="81"/>
+      <c r="C45" s="86" t="s">
         <v>100</v>
       </c>
       <c r="D45" s="11" t="s">
@@ -2921,8 +4181,8 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="2"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="68"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="84"/>
       <c r="D46" s="17" t="s">
         <v>16</v>
       </c>
@@ -2936,8 +4196,8 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="2"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="66" t="s">
+      <c r="B47" s="81"/>
+      <c r="C47" s="83" t="s">
         <v>106</v>
       </c>
       <c r="D47" s="16" t="s">
@@ -2953,8 +4213,8 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="2"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="68"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="84"/>
       <c r="D48" s="17" t="s">
         <v>108</v>
       </c>
@@ -2968,7 +4228,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2"/>
-      <c r="B49" s="62"/>
+      <c r="B49" s="81"/>
       <c r="C49" s="15" t="s">
         <v>109</v>
       </c>
@@ -2985,8 +4245,8 @@
     </row>
     <row r="50" spans="1:7" ht="25.5">
       <c r="A50" s="2"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="67" t="s">
+      <c r="B50" s="81"/>
+      <c r="C50" s="86" t="s">
         <v>113</v>
       </c>
       <c r="D50" s="11" t="s">
@@ -3002,8 +4262,8 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="67"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="86"/>
       <c r="D51" s="11" t="s">
         <v>16</v>
       </c>
@@ -3017,8 +4277,8 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="2"/>
-      <c r="B52" s="62"/>
-      <c r="C52" s="67"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="86"/>
       <c r="D52" s="11" t="s">
         <v>16</v>
       </c>
@@ -3032,8 +4292,8 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="69"/>
+      <c r="B53" s="82"/>
+      <c r="C53" s="87"/>
       <c r="D53" s="22" t="s">
         <v>16</v>
       </c>
@@ -3047,7 +4307,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2"/>
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="85" t="s">
         <v>119</v>
       </c>
       <c r="C54" s="9"/>
@@ -3058,8 +4318,8 @@
     </row>
     <row r="55" spans="1:7" ht="12.75" customHeight="1">
       <c r="A55" s="2"/>
-      <c r="B55" s="62"/>
-      <c r="C55" s="64" t="s">
+      <c r="B55" s="81"/>
+      <c r="C55" s="88" t="s">
         <v>120</v>
       </c>
       <c r="D55" s="11" t="s">
@@ -3075,8 +4335,8 @@
     </row>
     <row r="56" spans="1:7" ht="12.75" customHeight="1">
       <c r="A56" s="2"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="64"/>
+      <c r="B56" s="81"/>
+      <c r="C56" s="88"/>
       <c r="D56" s="11" t="s">
         <v>16</v>
       </c>
@@ -3090,8 +4350,8 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="2"/>
-      <c r="B57" s="62"/>
-      <c r="C57" s="65"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="89"/>
       <c r="D57" s="17" t="s">
         <v>125</v>
       </c>
@@ -3105,7 +4365,7 @@
     </row>
     <row r="58" spans="1:7" ht="25.5">
       <c r="A58" s="2"/>
-      <c r="B58" s="62"/>
+      <c r="B58" s="81"/>
       <c r="C58" s="13" t="s">
         <v>127</v>
       </c>
@@ -3120,7 +4380,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2"/>
-      <c r="B59" s="62"/>
+      <c r="B59" s="81"/>
       <c r="C59" s="13" t="s">
         <v>128</v>
       </c>
@@ -3135,8 +4395,8 @@
     </row>
     <row r="60" spans="1:7" ht="12.75" customHeight="1">
       <c r="A60" s="2"/>
-      <c r="B60" s="62"/>
-      <c r="C60" s="66" t="s">
+      <c r="B60" s="81"/>
+      <c r="C60" s="83" t="s">
         <v>129</v>
       </c>
       <c r="D60" s="16" t="s">
@@ -3152,8 +4412,8 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="2"/>
-      <c r="B61" s="62"/>
-      <c r="C61" s="67"/>
+      <c r="B61" s="81"/>
+      <c r="C61" s="86"/>
       <c r="D61" s="11" t="s">
         <v>131</v>
       </c>
@@ -3167,8 +4427,8 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="2"/>
-      <c r="B62" s="62"/>
-      <c r="C62" s="68"/>
+      <c r="B62" s="81"/>
+      <c r="C62" s="84"/>
       <c r="D62" s="17" t="s">
         <v>133</v>
       </c>
@@ -3182,8 +4442,8 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="2"/>
-      <c r="B63" s="62"/>
-      <c r="C63" s="67" t="s">
+      <c r="B63" s="81"/>
+      <c r="C63" s="86" t="s">
         <v>135</v>
       </c>
       <c r="D63" s="11" t="s">
@@ -3199,8 +4459,8 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="2"/>
-      <c r="B64" s="62"/>
-      <c r="C64" s="67"/>
+      <c r="B64" s="81"/>
+      <c r="C64" s="86"/>
       <c r="D64" s="11" t="s">
         <v>16</v>
       </c>
@@ -3214,8 +4474,8 @@
     </row>
     <row r="65" spans="1:7" ht="38.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="63"/>
-      <c r="C65" s="69"/>
+      <c r="B65" s="82"/>
+      <c r="C65" s="87"/>
       <c r="D65" s="30" t="s">
         <v>25</v>
       </c>
@@ -3427,13 +4687,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:B14"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B15:B25"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C25"/>
     <mergeCell ref="B54:B65"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="C60:C62"/>
@@ -3447,6 +4700,13 @@
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="C50:C53"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B15:B25"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3455,7 +4715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E62"/>
   <sheetViews>
@@ -3476,10 +4736,10 @@
     </row>
     <row r="2" spans="1:5" ht="13.5" thickBot="1">
       <c r="A2" s="53"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="72"/>
+      <c r="C2" s="79"/>
       <c r="D2" s="57" t="s">
         <v>142</v>
       </c>
@@ -3487,7 +4747,7 @@
     </row>
     <row r="3" spans="1:5" ht="13.5" thickTop="1">
       <c r="A3" s="53"/>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="80" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="6"/>
@@ -3496,7 +4756,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="53"/>
-      <c r="B4" s="62"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
@@ -3507,7 +4767,7 @@
     </row>
     <row r="5" spans="1:5" ht="25.5">
       <c r="A5" s="53"/>
-      <c r="B5" s="62"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
@@ -3518,8 +4778,8 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="53"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="66" t="s">
+      <c r="B6" s="81"/>
+      <c r="C6" s="83" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="24" t="s">
@@ -3529,8 +4789,8 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="53"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="68"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="29" t="s">
         <v>17</v>
       </c>
@@ -3538,8 +4798,8 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="53"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="66" t="s">
+      <c r="B8" s="81"/>
+      <c r="C8" s="83" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="24" t="s">
@@ -3549,8 +4809,8 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="53"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="68"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="29" t="s">
         <v>21</v>
       </c>
@@ -3558,7 +4818,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="53"/>
-      <c r="B10" s="62"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="15" t="s">
         <v>153</v>
       </c>
@@ -3569,7 +4829,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="53"/>
-      <c r="B11" s="63"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="21" t="s">
         <v>154</v>
       </c>
@@ -3580,7 +4840,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="53"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="85" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="54"/>
@@ -3589,7 +4849,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="53"/>
-      <c r="B13" s="62"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="18" t="s">
         <v>28</v>
       </c>
@@ -3600,8 +4860,8 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="53"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="66" t="s">
+      <c r="B14" s="81"/>
+      <c r="C14" s="83" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="24" t="s">
@@ -3611,8 +4871,8 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="53"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="67"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="10" t="s">
         <v>158</v>
       </c>
@@ -3620,8 +4880,8 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="53"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="68"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="84"/>
       <c r="D16" s="29" t="s">
         <v>157</v>
       </c>
@@ -3629,8 +4889,8 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="53"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="67" t="s">
+      <c r="B17" s="81"/>
+      <c r="C17" s="86" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -3640,8 +4900,8 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="53"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="67"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="10" t="s">
         <v>46</v>
       </c>
@@ -3649,8 +4909,8 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="53"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="67"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="10" t="s">
         <v>48</v>
       </c>
@@ -3658,8 +4918,8 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="53"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="69"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="87"/>
       <c r="D20" s="26" t="s">
         <v>159</v>
       </c>
@@ -3667,7 +4927,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="53"/>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="85" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="23"/>
@@ -3676,7 +4936,7 @@
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1">
       <c r="A22" s="53"/>
-      <c r="B22" s="62"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="23" t="s">
         <v>53</v>
       </c>
@@ -3687,7 +4947,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="53"/>
-      <c r="B23" s="62"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="15" t="s">
         <v>63</v>
       </c>
@@ -3698,8 +4958,8 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="53"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="67" t="s">
+      <c r="B24" s="81"/>
+      <c r="C24" s="86" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="10">
@@ -3709,8 +4969,8 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="53"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="67"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="86"/>
       <c r="D25" s="10" t="s">
         <v>145</v>
       </c>
@@ -3718,8 +4978,8 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="53"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="67"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="10" t="s">
         <v>143</v>
       </c>
@@ -3727,8 +4987,8 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="53"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="67"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="10" t="s">
         <v>146</v>
       </c>
@@ -3736,8 +4996,8 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="53"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="69"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="87"/>
       <c r="D28" s="26" t="s">
         <v>144</v>
       </c>
@@ -3745,7 +5005,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="53"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="85" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="9"/>
@@ -3754,14 +5014,14 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="53"/>
-      <c r="B30" s="62"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
       <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="53"/>
-      <c r="B31" s="62"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="59" t="s">
         <v>162</v>
       </c>
@@ -3772,8 +5032,8 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="53"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="64" t="s">
+      <c r="B32" s="81"/>
+      <c r="C32" s="88" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -3783,8 +5043,8 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="53"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="64"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="88"/>
       <c r="D33" s="10" t="s">
         <v>81</v>
       </c>
@@ -3792,8 +5052,8 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="53"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="64"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="88"/>
       <c r="D34" s="10" t="s">
         <v>161</v>
       </c>
@@ -3801,8 +5061,8 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="53"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="64"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="88"/>
       <c r="D35" s="10" t="s">
         <v>84</v>
       </c>
@@ -3810,8 +5070,8 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="53"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="65"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="89"/>
       <c r="D36" s="29" t="s">
         <v>85</v>
       </c>
@@ -3819,7 +5079,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="53"/>
-      <c r="B37" s="62"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="19" t="s">
         <v>164</v>
       </c>
@@ -3830,7 +5090,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="53"/>
-      <c r="B38" s="62"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="13" t="s">
         <v>87</v>
       </c>
@@ -3841,7 +5101,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="53"/>
-      <c r="B39" s="62"/>
+      <c r="B39" s="81"/>
       <c r="C39" s="13" t="s">
         <v>91</v>
       </c>
@@ -3852,7 +5112,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="53"/>
-      <c r="B40" s="63"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="27" t="s">
         <v>95</v>
       </c>
@@ -3863,7 +5123,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="53"/>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="85" t="s">
         <v>99</v>
       </c>
       <c r="C41" s="23"/>
@@ -3872,7 +5132,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="53"/>
-      <c r="B42" s="62"/>
+      <c r="B42" s="81"/>
       <c r="C42" s="23" t="s">
         <v>148</v>
       </c>
@@ -3883,8 +5143,8 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="53"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="66" t="s">
+      <c r="B43" s="81"/>
+      <c r="C43" s="83" t="s">
         <v>106</v>
       </c>
       <c r="D43" s="24" t="s">
@@ -3894,8 +5154,8 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="53"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="68"/>
+      <c r="B44" s="81"/>
+      <c r="C44" s="84"/>
       <c r="D44" s="29" t="s">
         <v>108</v>
       </c>
@@ -3903,7 +5163,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="53"/>
-      <c r="B45" s="62"/>
+      <c r="B45" s="81"/>
       <c r="C45" s="15" t="s">
         <v>109</v>
       </c>
@@ -3914,8 +5174,8 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="53"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="67" t="s">
+      <c r="B46" s="81"/>
+      <c r="C46" s="86" t="s">
         <v>113</v>
       </c>
       <c r="D46" s="10" t="s">
@@ -3925,8 +5185,8 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="53"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="67"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="86"/>
       <c r="D47" s="10" t="s">
         <v>115</v>
       </c>
@@ -3934,8 +5194,8 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="53"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="67"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="86"/>
       <c r="D48" s="10" t="s">
         <v>117</v>
       </c>
@@ -3943,8 +5203,8 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="53"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="69"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="87"/>
       <c r="D49" s="26" t="s">
         <v>118</v>
       </c>
@@ -3952,7 +5212,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="53"/>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="85" t="s">
         <v>119</v>
       </c>
       <c r="C50" s="9"/>
@@ -3961,8 +5221,8 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="53"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="64" t="s">
+      <c r="B51" s="81"/>
+      <c r="C51" s="88" t="s">
         <v>120</v>
       </c>
       <c r="D51" s="10" t="s">
@@ -3972,8 +5232,8 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="53"/>
-      <c r="B52" s="62"/>
-      <c r="C52" s="64"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="88"/>
       <c r="D52" s="10" t="s">
         <v>123</v>
       </c>
@@ -3981,7 +5241,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="53"/>
-      <c r="B53" s="62"/>
+      <c r="B53" s="81"/>
       <c r="C53" s="13" t="s">
         <v>151</v>
       </c>
@@ -3992,8 +5252,8 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="53"/>
-      <c r="B54" s="62"/>
-      <c r="C54" s="66" t="s">
+      <c r="B54" s="81"/>
+      <c r="C54" s="83" t="s">
         <v>129</v>
       </c>
       <c r="D54" s="24" t="s">
@@ -4003,8 +5263,8 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="53"/>
-      <c r="B55" s="62"/>
-      <c r="C55" s="67"/>
+      <c r="B55" s="81"/>
+      <c r="C55" s="86"/>
       <c r="D55" s="10" t="s">
         <v>131</v>
       </c>
@@ -4012,8 +5272,8 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="53"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="68"/>
+      <c r="B56" s="81"/>
+      <c r="C56" s="84"/>
       <c r="D56" s="29" t="s">
         <v>133</v>
       </c>
@@ -4021,8 +5281,8 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="53"/>
-      <c r="B57" s="62"/>
-      <c r="C57" s="67" t="s">
+      <c r="B57" s="81"/>
+      <c r="C57" s="86" t="s">
         <v>135</v>
       </c>
       <c r="D57" s="10" t="s">
@@ -4032,8 +5292,8 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="53"/>
-      <c r="B58" s="62"/>
-      <c r="C58" s="67"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="86"/>
       <c r="D58" s="10" t="s">
         <v>137</v>
       </c>
@@ -4041,8 +5301,8 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="53"/>
-      <c r="B59" s="63"/>
-      <c r="C59" s="69"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="87"/>
       <c r="D59" s="26" t="s">
         <v>138</v>
       </c>
@@ -4061,13 +5321,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B12:B20"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C20"/>
     <mergeCell ref="B50:B59"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C54:C56"/>
@@ -4079,18 +5332,25 @@
     <mergeCell ref="B41:B49"/>
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="C46:C49"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B12:B20"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G15"/>
+  <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4103,213 +5363,265 @@
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="B2" s="74" t="s">
+    <row r="2" spans="1:8">
+      <c r="B2" s="61" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="73" t="s">
         <v>173</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="67" t="s">
         <v>170</v>
       </c>
-      <c r="E4" s="79" t="s">
+      <c r="E4" s="66" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="F4" s="67" t="s">
         <v>168</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="70" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="85" t="s">
+      <c r="H4" s="91" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="C5" s="67" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="D5" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="71"/>
+      <c r="F5" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="D5" s="87" t="s">
-        <v>176</v>
-      </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="87" t="s">
+      <c r="G5" s="67" t="s">
         <v>177</v>
       </c>
-      <c r="G5" s="80" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15">
-      <c r="B6" s="81">
+      <c r="H5" s="91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15">
+      <c r="B6" s="68">
         <v>4</v>
       </c>
-      <c r="C6" s="81">
+      <c r="C6" s="68">
         <v>4</v>
       </c>
-      <c r="D6" s="81">
+      <c r="D6" s="68">
         <v>1024</v>
       </c>
-      <c r="E6" s="75">
+      <c r="E6" s="62">
         <v>1847</v>
       </c>
-      <c r="F6" s="81">
+      <c r="F6" s="68">
         <v>200000000</v>
       </c>
-      <c r="G6" s="89">
+      <c r="G6" s="76">
         <f>((D6*B6)/E6)*F6</f>
         <v>443530048.7276665</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="81"/>
-      <c r="C7" s="81">
+      <c r="H6" s="92">
+        <f>G6/1000000</f>
+        <v>443.5300487276665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="68"/>
+      <c r="C7" s="68">
         <v>5</v>
       </c>
-      <c r="D7" s="81"/>
-      <c r="E7" s="76">
+      <c r="D7" s="68"/>
+      <c r="E7" s="63">
         <v>1600</v>
       </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="88">
+      <c r="F7" s="68"/>
+      <c r="G7" s="75">
         <f>((D6*B6)/E7)*F6</f>
         <v>512000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="81"/>
-      <c r="C8" s="81">
+      <c r="H7" s="92">
+        <f t="shared" ref="H7:H15" si="0">G7/1000000</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" s="68"/>
+      <c r="C8" s="68">
         <v>6</v>
       </c>
-      <c r="D8" s="81"/>
-      <c r="E8" s="76">
+      <c r="D8" s="68"/>
+      <c r="E8" s="63">
         <v>1185</v>
       </c>
-      <c r="F8" s="81"/>
-      <c r="G8" s="88">
+      <c r="F8" s="68"/>
+      <c r="G8" s="75">
         <f>((D6*B6)/E8)*F6</f>
         <v>691308016.87763715</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="81"/>
-      <c r="C9" s="81">
+      <c r="H8" s="92">
+        <f t="shared" si="0"/>
+        <v>691.3080168776371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" s="68"/>
+      <c r="C9" s="68">
         <v>7</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="76">
+      <c r="D9" s="68"/>
+      <c r="E9" s="63">
         <v>1168</v>
       </c>
-      <c r="F9" s="81"/>
-      <c r="G9" s="88">
+      <c r="F9" s="68"/>
+      <c r="G9" s="75">
         <f>((D6*B6)/E9)*F6</f>
         <v>701369863.01369858</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="81"/>
-      <c r="C10" s="81">
+      <c r="H9" s="92">
+        <f t="shared" si="0"/>
+        <v>701.36986301369859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" s="68"/>
+      <c r="C10" s="68">
         <v>8</v>
       </c>
-      <c r="D10" s="81"/>
-      <c r="E10" s="76">
+      <c r="D10" s="68"/>
+      <c r="E10" s="63">
         <v>1181</v>
       </c>
-      <c r="F10" s="81"/>
-      <c r="G10" s="88">
+      <c r="F10" s="68"/>
+      <c r="G10" s="75">
         <f>((D6*B6)/E10)*F6</f>
         <v>693649449.61896694</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="81"/>
-      <c r="C11" s="81">
+      <c r="H10" s="92">
+        <f t="shared" si="0"/>
+        <v>693.64944961896697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="68"/>
+      <c r="C11" s="68">
         <v>9</v>
       </c>
-      <c r="D11" s="81"/>
-      <c r="E11" s="76">
+      <c r="D11" s="68"/>
+      <c r="E11" s="63">
         <v>1180</v>
       </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="88">
+      <c r="F11" s="68"/>
+      <c r="G11" s="75">
         <f>((D6*B6)/E11)*F6</f>
         <v>694237288.13559318</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="81"/>
-      <c r="C12" s="81">
+      <c r="H11" s="92">
+        <f t="shared" si="0"/>
+        <v>694.23728813559319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" s="68"/>
+      <c r="C12" s="68">
         <v>10</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="76">
+      <c r="D12" s="68"/>
+      <c r="E12" s="63">
         <v>1167</v>
       </c>
-      <c r="F12" s="81"/>
-      <c r="G12" s="88">
+      <c r="F12" s="68"/>
+      <c r="G12" s="75">
         <f>((D6*B6)/E12)*F6</f>
         <v>701970865.46700943</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="81"/>
-      <c r="C13" s="81">
+      <c r="H12" s="92">
+        <f t="shared" si="0"/>
+        <v>701.97086546700939</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" s="68"/>
+      <c r="C13" s="68">
         <v>11</v>
       </c>
-      <c r="D13" s="81"/>
-      <c r="E13" s="76">
+      <c r="D13" s="68"/>
+      <c r="E13" s="63">
         <v>1175</v>
       </c>
-      <c r="F13" s="81"/>
-      <c r="G13" s="88">
+      <c r="F13" s="68"/>
+      <c r="G13" s="75">
         <f>((D6*B6)/E13)*F6</f>
         <v>697191489.36170208</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="81"/>
-      <c r="C14" s="81">
+      <c r="H13" s="92">
+        <f t="shared" si="0"/>
+        <v>697.19148936170211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="68"/>
+      <c r="C14" s="68">
         <v>64</v>
       </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="76">
+      <c r="D14" s="68"/>
+      <c r="E14" s="63">
         <v>1114</v>
       </c>
-      <c r="F14" s="81"/>
-      <c r="G14" s="88">
+      <c r="F14" s="68"/>
+      <c r="G14" s="75">
         <f>((D6*B6)/E14)*F6</f>
         <v>735368043.08797133</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15">
-      <c r="B15" s="82"/>
-      <c r="C15" s="82">
+      <c r="H14" s="92">
+        <f t="shared" si="0"/>
+        <v>735.36804308797127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69">
         <v>256</v>
       </c>
-      <c r="D15" s="82"/>
-      <c r="E15" s="77">
+      <c r="D15" s="69"/>
+      <c r="E15" s="64">
         <v>1077</v>
       </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="90">
+      <c r="F15" s="69"/>
+      <c r="G15" s="77">
         <f>((D6*B6)/E15)*F6</f>
         <v>760631383.47260904</v>
       </c>
+      <c r="H15" s="92">
+        <f t="shared" si="0"/>
+        <v>760.63138347260906</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="61" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>